<commit_message>
Added JSON Files required for AllianzTesting and Added server timeout in app.config
</commit_message>
<xml_diff>
--- a/TestDataMapper/bin/Debug/XPathMapper.xlsx
+++ b/TestDataMapper/bin/Debug/XPathMapper.xlsx
@@ -5,47 +5,37 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TestDataMapper_GitHub\TestDataMapper\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Saket_Latest\TestDataMapper\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F051A43A-6ABE-4A84-9060-56C9512AEAD2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93DE21C-8984-413D-8C20-5BE895D70191}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
-  <si>
-    <t>Vehicle Class</t>
-  </si>
-  <si>
-    <t>Use</t>
-  </si>
-  <si>
-    <t>Other Insurance</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="72">
   <si>
     <t>Gender</t>
   </si>
   <si>
-    <t>Driver Age</t>
-  </si>
-  <si>
     <t>NVIC</t>
   </si>
   <si>
-    <t>Vehicle Age</t>
-  </si>
-  <si>
-    <t>KM</t>
-  </si>
-  <si>
     <t>DemeritPoints</t>
   </si>
   <si>
@@ -64,9 +54,6 @@
     <t>RegistrationDueDate</t>
   </si>
   <si>
-    <t>RegistrationDueYear</t>
-  </si>
-  <si>
     <t>YearOfManufacture</t>
   </si>
   <si>
@@ -88,15 +75,9 @@
     <t>Input</t>
   </si>
   <si>
-    <t>IndividualOrCompany</t>
-  </si>
-  <si>
     <t>session/data/policy/line/risk/CompanyOwned</t>
   </si>
   <si>
-    <t>Driver History</t>
-  </si>
-  <si>
     <t>session/data/policy/line/risk/Use</t>
   </si>
   <si>
@@ -112,24 +93,15 @@
     <t>Shape</t>
   </si>
   <si>
-    <t>session/data/policy/line/risk/Shape</t>
-  </si>
-  <si>
     <t>Make</t>
   </si>
   <si>
-    <t>session/data/policy/line/risk/MakeCode</t>
-  </si>
-  <si>
     <t>session/data/policy/line/risk/YearOfManufacture</t>
   </si>
   <si>
     <t>session/data/policy/line/risk/Kilometers</t>
   </si>
   <si>
-    <t>Premium</t>
-  </si>
-  <si>
     <t>ITC</t>
   </si>
   <si>
@@ -190,9 +162,6 @@
     <t>session/data/policy/line/Comparer/Allianz/Allianz6MonthsPremium/TotalPremium</t>
   </si>
   <si>
-    <t>VehGarageCd</t>
-  </si>
-  <si>
     <t>session/data/policy/line/risk/VehGarageCd</t>
   </si>
   <si>
@@ -202,13 +171,79 @@
     <t>session/data/policy/line/risk/RegistrationDueDate</t>
   </si>
   <si>
-    <t>CalculationInput</t>
-  </si>
-  <si>
-    <t>split([RegistrationDueDate],0,4)</t>
-  </si>
-  <si>
-    <t>diff([RegistrationDueYear],[Vehicle Age])</t>
+    <t>Vehicle_Type</t>
+  </si>
+  <si>
+    <t>Individual_Or_Company</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>session/data/policy/line/risk/Model</t>
+  </si>
+  <si>
+    <t>session/data/policy/line/risk/Make</t>
+  </si>
+  <si>
+    <t>session/data/policy/line/risk/VehicleShape</t>
+  </si>
+  <si>
+    <t>REGION</t>
+  </si>
+  <si>
+    <t>Kilometers</t>
+  </si>
+  <si>
+    <t>Vehicle_Used_For</t>
+  </si>
+  <si>
+    <t>IsCurrentCTPGreenSlip</t>
+  </si>
+  <si>
+    <t>session/data/policy/line/risk/CurrentCTP</t>
+  </si>
+  <si>
+    <t>CurrentCTPCompany</t>
+  </si>
+  <si>
+    <t>session/data/policy/line/risk/CurrentCTPCompany</t>
+  </si>
+  <si>
+    <t>IsBlueSlipRequired</t>
+  </si>
+  <si>
+    <t>session/data/policy/line/risk/BlueSlip</t>
+  </si>
+  <si>
+    <t>Other_Motor_Insurance</t>
+  </si>
+  <si>
+    <t>OtherInsuranceCompany</t>
+  </si>
+  <si>
+    <t>session/data/policy/line/risk/OtherInsuranceCompany</t>
+  </si>
+  <si>
+    <t>Driver_Age</t>
+  </si>
+  <si>
+    <t>Pillion_Passenger</t>
+  </si>
+  <si>
+    <t>session/data/policy/line/driver/PillionPassenger</t>
+  </si>
+  <si>
+    <t>AnyConvictionsOrSuspensionInLast3Yrs</t>
+  </si>
+  <si>
+    <t>session/data/policy/line/driver/AnyConvictionsOrSuspensionInLast3Yrs</t>
+  </si>
+  <si>
+    <t>EngineCapacity</t>
+  </si>
+  <si>
+    <t>session/data/policy/line/risk/EngineCapacity</t>
   </si>
 </sst>
 </file>
@@ -290,23 +325,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81BAC6B5-E3F1-404C-89BB-BB810293EA0B}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,323 +686,380 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="B15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="57" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="C34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Code Changes for Write Excel and serverRequestType
</commit_message>
<xml_diff>
--- a/TestDataMapper/bin/Debug/XPathMapper.xlsx
+++ b/TestDataMapper/bin/Debug/XPathMapper.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaurav.sawadekar\Documents\SIRA DPR\YOUI\chaintanya given tool for request and response testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Saket_Latest\TestDataMapper\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46A8628-A756-437B-8D84-5BA41848AC62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5857EA95-3636-4177-8E09-A175FB2D1904}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="74">
   <si>
     <t>Gender</t>
   </si>
@@ -234,22 +234,22 @@
     <t>Kilometres</t>
   </si>
   <si>
-    <t>session/data/policy/line/Comparer/YOUI/YOUI12MonthsPremium/Premium</t>
-  </si>
-  <si>
-    <t>session/data/policy/line/Comparer/YOUI/YOUI12MonthsPremium/GST</t>
-  </si>
-  <si>
-    <t>session/data/policy/line/Comparer/YOUI/YOUI12MonthsPremium/TotalPremium</t>
-  </si>
-  <si>
-    <t>session/data/policy/line/Comparer/YOUI/YOUI6MonthsPremium/Premium</t>
-  </si>
-  <si>
-    <t>session/data/policy/line/Comparer/YOUI/YOUI6MonthsPremium/GST</t>
-  </si>
-  <si>
-    <t>session/data/policy/line/Comparer/YOUI/YOUI6MonthsPremium/TotalPremium</t>
+    <t>session/data/policy/line/Comparer/12MonthsPremium/Premium</t>
+  </si>
+  <si>
+    <t>session/data/policy/line/Comparer/12MonthsPremium/GST</t>
+  </si>
+  <si>
+    <t>session/data/policy/line/Comparer/12MonthsPremium/TotalPremium</t>
+  </si>
+  <si>
+    <t>session/data/policy/line/Comparer/6MonthsPremium/Premium</t>
+  </si>
+  <si>
+    <t>session/data/policy/line/Comparer/6MonthsPremium/GST</t>
+  </si>
+  <si>
+    <t>session/data/policy/line/Comparer/6MonthsPremium/TotalPremium</t>
   </si>
 </sst>
 </file>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81BAC6B5-E3F1-404C-89BB-BB810293EA0B}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,7 +734,9 @@
       <c r="B4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -862,9 +864,7 @@
       <c r="B16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
@@ -873,9 +873,7 @@
       <c r="B17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">

</xml_diff>